<commit_message>
Added additonal deployment details
</commit_message>
<xml_diff>
--- a/PreProd Refresh/Supporting Files/DeploymentDetails2.xlsx
+++ b/PreProd Refresh/Supporting Files/DeploymentDetails2.xlsx
@@ -12,8 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="Deployments" sheetId="1" r:id="rId1"/>
-    <sheet name="DBBackups" sheetId="2" r:id="rId2"/>
+    <sheet name="Deployments_9th" sheetId="4" r:id="rId1"/>
+    <sheet name="Deployments" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="DBBackups" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20180427\WUK.6690.30555\WUK.6690.30555</t>
   </si>
@@ -181,6 +183,24 @@
   </si>
   <si>
     <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20181001\VRUKL.6848.27222</t>
+  </si>
+  <si>
+    <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20180901\VRUKL.6817.28984</t>
+  </si>
+  <si>
+    <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20180918\VRUKL.6830.25880</t>
+  </si>
+  <si>
+    <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20180924\VRUKL.6838.24144</t>
+  </si>
+  <si>
+    <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20181002\VRUKL.6849.22911\VRUKL.6849.22911</t>
+  </si>
+  <si>
+    <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20180927\VRUKL.6844.22422</t>
+  </si>
+  <si>
+    <t>\\vrgefs01\shared\IT\Programme Victory\Releases\Web Apps\20181001\VRUKL.6848.24666</t>
   </si>
 </sst>
 </file>
@@ -532,9 +552,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="118.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -657,7 +768,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>

</xml_diff>